<commit_message>
fixed a few part numbers in the BOM and board
</commit_message>
<xml_diff>
--- a/hardware/battery_pack/rev_a/battery_pack_bom.xlsx
+++ b/hardware/battery_pack/rev_a/battery_pack_bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="97">
   <si>
     <t xml:space="preserve">Part</t>
   </si>
@@ -88,15 +88,9 @@
     <t xml:space="preserve">C2</t>
   </si>
   <si>
-    <t xml:space="preserve">312-1087-1-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">C3</t>
   </si>
   <si>
-    <t xml:space="preserve">313-1087-1-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">C4</t>
   </si>
   <si>
@@ -109,9 +103,6 @@
     <t xml:space="preserve">C5</t>
   </si>
   <si>
-    <t xml:space="preserve">312-1445-1-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">J1</t>
   </si>
   <si>
@@ -124,7 +115,7 @@
     <t xml:space="preserve">CP-102AH-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">Q3</t>
+    <t xml:space="preserve">Q1</t>
   </si>
   <si>
     <t xml:space="preserve">MOSFET-NCHANNELFDD8580</t>
@@ -139,7 +130,7 @@
     <t xml:space="preserve">FDD8447L_F085CT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">Q4</t>
+    <t xml:space="preserve">Q2</t>
   </si>
   <si>
     <t xml:space="preserve">R1</t>
@@ -178,27 +169,15 @@
     <t xml:space="preserve">R3</t>
   </si>
   <si>
-    <t xml:space="preserve">312-1.0KGRCT-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">R4</t>
   </si>
   <si>
-    <t xml:space="preserve">313-1.0KGRCT-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">R5</t>
   </si>
   <si>
-    <t xml:space="preserve">314-1.0KGRCT-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">R6</t>
   </si>
   <si>
-    <t xml:space="preserve">315-1.0KGRCT-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">R7</t>
   </si>
   <si>
@@ -245,9 +224,6 @@
   </si>
   <si>
     <t xml:space="preserve">R12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">312-1.0MGRCT-ND</t>
   </si>
   <si>
     <t xml:space="preserve">TP1</t>
@@ -349,6 +325,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -433,19 +410,19 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.9030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="26.8520408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.1428571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.3316326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4030612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.51530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -562,12 +539,12 @@
         <v>19</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>16</v>
@@ -582,15 +559,15 @@
         <v>19</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>17</v>
@@ -602,15 +579,15 @@
         <v>19</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>17</v>
@@ -622,630 +599,630 @@
         <v>19</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="F11" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.016</v>
       </c>
       <c r="C13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="E14" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="F14" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="F15" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="F16" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="F17" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="F18" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>